<commit_message>
Siri Bhoovalya play ground in  Handy Excel File for Dummies
</commit_message>
<xml_diff>
--- a/SiriBhoovalaya.xlsx
+++ b/SiriBhoovalaya.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rama\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\Siri\SiriBhoovalaya\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7395"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7395" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Straight_5x5" sheetId="1" r:id="rId1"/>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +851,7 @@
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1227,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE88"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:AC59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,6 +1236,7 @@
     <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="29" width="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -10277,8 +10278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE88"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10286,6 +10287,7 @@
     <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="29" width="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -14375,7 +14377,7 @@
       </c>
       <c r="D62" s="1">
         <f t="shared" ref="D62:AC62" ca="1" si="7">IFERROR(CODE(LOWER(D33)),RANDBETWEEN(1,729))</f>
-        <v>206</v>
+        <v>551</v>
       </c>
       <c r="E62" s="1">
         <f t="shared" ca="1" si="7"/>
@@ -14391,7 +14393,7 @@
       </c>
       <c r="H62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>683</v>
+        <v>639</v>
       </c>
       <c r="I62" s="1">
         <f t="shared" ca="1" si="7"/>
@@ -14407,7 +14409,7 @@
       </c>
       <c r="L62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>566</v>
+        <v>355</v>
       </c>
       <c r="M62" s="1">
         <f t="shared" ca="1" si="7"/>
@@ -14415,67 +14417,67 @@
       </c>
       <c r="N62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="O62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>385</v>
+        <v>225</v>
       </c>
       <c r="P62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>578</v>
+        <v>363</v>
       </c>
       <c r="Q62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>165</v>
+        <v>697</v>
       </c>
       <c r="R62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>370</v>
+        <v>298</v>
       </c>
       <c r="S62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>489</v>
+        <v>227</v>
       </c>
       <c r="T62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="U62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>234</v>
+        <v>589</v>
       </c>
       <c r="V62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>82</v>
+        <v>672</v>
       </c>
       <c r="W62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>126</v>
+        <v>559</v>
       </c>
       <c r="X62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>379</v>
+        <v>434</v>
       </c>
       <c r="Y62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Z62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>359</v>
+        <v>490</v>
       </c>
       <c r="AA62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>496</v>
+        <v>610</v>
       </c>
       <c r="AB62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>73</v>
+        <v>231</v>
       </c>
       <c r="AC62" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>121</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.25">
@@ -14485,7 +14487,7 @@
       </c>
       <c r="D63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>252</v>
+        <v>516</v>
       </c>
       <c r="E63" s="1">
         <f t="shared" ca="1" si="8"/>
@@ -14493,7 +14495,7 @@
       </c>
       <c r="F63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>368</v>
+        <v>478</v>
       </c>
       <c r="G63" s="1">
         <f t="shared" ca="1" si="8"/>
@@ -14501,7 +14503,7 @@
       </c>
       <c r="H63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>551</v>
+        <v>351</v>
       </c>
       <c r="I63" s="1">
         <f t="shared" ca="1" si="8"/>
@@ -14509,7 +14511,7 @@
       </c>
       <c r="J63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>231</v>
+        <v>422</v>
       </c>
       <c r="K63" s="1">
         <f t="shared" ca="1" si="8"/>
@@ -14517,7 +14519,7 @@
       </c>
       <c r="L63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>298</v>
+        <v>549</v>
       </c>
       <c r="M63" s="1">
         <f t="shared" ca="1" si="8"/>
@@ -14525,67 +14527,67 @@
       </c>
       <c r="N63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>708</v>
+        <v>501</v>
       </c>
       <c r="O63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="P63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>503</v>
       </c>
       <c r="Q63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>579</v>
+        <v>45</v>
       </c>
       <c r="R63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="S63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>512</v>
+        <v>424</v>
       </c>
       <c r="T63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>231</v>
+        <v>554</v>
       </c>
       <c r="U63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>240</v>
+        <v>507</v>
       </c>
       <c r="V63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>114</v>
+        <v>537</v>
       </c>
       <c r="W63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="X63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>713</v>
+        <v>386</v>
       </c>
       <c r="Y63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>91</v>
+        <v>264</v>
       </c>
       <c r="Z63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>622</v>
+        <v>395</v>
       </c>
       <c r="AA63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>434</v>
+        <v>52</v>
       </c>
       <c r="AB63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>30</v>
+        <v>599</v>
       </c>
       <c r="AC63" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>163</v>
+        <v>726</v>
       </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.25">
@@ -14595,7 +14597,7 @@
       </c>
       <c r="D64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>653</v>
+        <v>539</v>
       </c>
       <c r="E64" s="1">
         <f t="shared" ca="1" si="9"/>
@@ -14603,7 +14605,7 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>416</v>
+        <v>580</v>
       </c>
       <c r="G64" s="1">
         <f t="shared" ca="1" si="9"/>
@@ -14611,7 +14613,7 @@
       </c>
       <c r="H64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>592</v>
+        <v>685</v>
       </c>
       <c r="I64" s="1">
         <f t="shared" ca="1" si="9"/>
@@ -14619,7 +14621,7 @@
       </c>
       <c r="J64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>271</v>
+        <v>394</v>
       </c>
       <c r="K64" s="1">
         <f t="shared" ca="1" si="9"/>
@@ -14627,7 +14629,7 @@
       </c>
       <c r="L64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>244</v>
+        <v>283</v>
       </c>
       <c r="M64" s="1">
         <f t="shared" ca="1" si="9"/>
@@ -14635,67 +14637,67 @@
       </c>
       <c r="N64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>678</v>
+        <v>129</v>
       </c>
       <c r="O64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>282</v>
+        <v>479</v>
       </c>
       <c r="P64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>619</v>
+        <v>42</v>
       </c>
       <c r="Q64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>651</v>
+        <v>74</v>
       </c>
       <c r="R64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>498</v>
+        <v>361</v>
       </c>
       <c r="S64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>602</v>
+        <v>374</v>
       </c>
       <c r="T64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>308</v>
+        <v>464</v>
       </c>
       <c r="U64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>397</v>
+        <v>553</v>
       </c>
       <c r="V64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>397</v>
+        <v>59</v>
       </c>
       <c r="W64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>355</v>
+        <v>120</v>
       </c>
       <c r="X64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>307</v>
+        <v>222</v>
       </c>
       <c r="Y64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>556</v>
+        <v>117</v>
       </c>
       <c r="Z64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>429</v>
+        <v>547</v>
       </c>
       <c r="AA64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>42</v>
+        <v>329</v>
       </c>
       <c r="AB64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>410</v>
+        <v>33</v>
       </c>
       <c r="AC64" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>195</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="3:29" x14ac:dyDescent="0.25">
@@ -14705,7 +14707,7 @@
       </c>
       <c r="D65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>246</v>
+        <v>490</v>
       </c>
       <c r="E65" s="1">
         <f t="shared" ca="1" si="10"/>
@@ -14713,7 +14715,7 @@
       </c>
       <c r="F65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="G65" s="1">
         <f t="shared" ca="1" si="10"/>
@@ -14721,7 +14723,7 @@
       </c>
       <c r="H65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>681</v>
+        <v>200</v>
       </c>
       <c r="I65" s="1">
         <f t="shared" ca="1" si="10"/>
@@ -14729,7 +14731,7 @@
       </c>
       <c r="J65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="K65" s="1">
         <f t="shared" ca="1" si="10"/>
@@ -14737,7 +14739,7 @@
       </c>
       <c r="L65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>146</v>
+        <v>235</v>
       </c>
       <c r="M65" s="1">
         <f t="shared" ca="1" si="10"/>
@@ -14745,67 +14747,67 @@
       </c>
       <c r="N65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>701</v>
+        <v>49</v>
       </c>
       <c r="O65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="P65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>47</v>
+        <v>627</v>
       </c>
       <c r="Q65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>300</v>
+        <v>595</v>
       </c>
       <c r="R65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>10</v>
+        <v>527</v>
       </c>
       <c r="S65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>627</v>
+        <v>81</v>
       </c>
       <c r="T65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>69</v>
+        <v>701</v>
       </c>
       <c r="U65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="V65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>57</v>
+        <v>199</v>
       </c>
       <c r="W65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>470</v>
+        <v>62</v>
       </c>
       <c r="X65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>376</v>
+        <v>711</v>
       </c>
       <c r="Y65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="Z65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>152</v>
+        <v>198</v>
       </c>
       <c r="AA65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>624</v>
+        <v>5</v>
       </c>
       <c r="AB65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>678</v>
+        <v>86</v>
       </c>
       <c r="AC65" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>273</v>
+        <v>309</v>
       </c>
     </row>
     <row r="66" spans="3:29" x14ac:dyDescent="0.25">
@@ -14815,7 +14817,7 @@
       </c>
       <c r="D66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>388</v>
+        <v>205</v>
       </c>
       <c r="E66" s="1">
         <f t="shared" ca="1" si="11"/>
@@ -14823,7 +14825,7 @@
       </c>
       <c r="F66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>651</v>
+        <v>484</v>
       </c>
       <c r="G66" s="1">
         <f t="shared" ca="1" si="11"/>
@@ -14831,7 +14833,7 @@
       </c>
       <c r="H66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>441</v>
+        <v>133</v>
       </c>
       <c r="I66" s="1">
         <f t="shared" ca="1" si="11"/>
@@ -14839,7 +14841,7 @@
       </c>
       <c r="J66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>495</v>
+        <v>400</v>
       </c>
       <c r="K66" s="1">
         <f t="shared" ca="1" si="11"/>
@@ -14847,7 +14849,7 @@
       </c>
       <c r="L66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>710</v>
+        <v>25</v>
       </c>
       <c r="M66" s="1">
         <f t="shared" ca="1" si="11"/>
@@ -14855,67 +14857,67 @@
       </c>
       <c r="N66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>533</v>
+        <v>207</v>
       </c>
       <c r="O66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>586</v>
+        <v>101</v>
       </c>
       <c r="P66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>153</v>
+        <v>215</v>
       </c>
       <c r="Q66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>39</v>
+        <v>430</v>
       </c>
       <c r="R66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>631</v>
+        <v>64</v>
       </c>
       <c r="S66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>91</v>
+        <v>359</v>
       </c>
       <c r="T66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>291</v>
+        <v>123</v>
       </c>
       <c r="U66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>610</v>
+        <v>589</v>
       </c>
       <c r="V66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>580</v>
+        <v>75</v>
       </c>
       <c r="W66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>402</v>
+        <v>189</v>
       </c>
       <c r="X66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>235</v>
+        <v>617</v>
       </c>
       <c r="Y66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>298</v>
+        <v>472</v>
       </c>
       <c r="Z66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>434</v>
+        <v>110</v>
       </c>
       <c r="AA66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>380</v>
+        <v>1</v>
       </c>
       <c r="AB66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>626</v>
+        <v>155</v>
       </c>
       <c r="AC66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>368</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="3:29" x14ac:dyDescent="0.25">
@@ -14925,7 +14927,7 @@
       </c>
       <c r="D67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>192</v>
+        <v>617</v>
       </c>
       <c r="E67" s="1">
         <f t="shared" ca="1" si="12"/>
@@ -14933,7 +14935,7 @@
       </c>
       <c r="F67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>570</v>
+        <v>391</v>
       </c>
       <c r="G67" s="1">
         <f t="shared" ca="1" si="12"/>
@@ -14941,7 +14943,7 @@
       </c>
       <c r="H67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>601</v>
+        <v>571</v>
       </c>
       <c r="I67" s="1">
         <f t="shared" ca="1" si="12"/>
@@ -14949,7 +14951,7 @@
       </c>
       <c r="J67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>364</v>
+        <v>25</v>
       </c>
       <c r="K67" s="1">
         <f t="shared" ca="1" si="12"/>
@@ -14957,7 +14959,7 @@
       </c>
       <c r="L67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>193</v>
+        <v>327</v>
       </c>
       <c r="M67" s="1">
         <f t="shared" ca="1" si="12"/>
@@ -14965,67 +14967,67 @@
       </c>
       <c r="N67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>4</v>
+        <v>394</v>
       </c>
       <c r="O67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>298</v>
+        <v>596</v>
       </c>
       <c r="P67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>594</v>
+        <v>60</v>
       </c>
       <c r="Q67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>344</v>
+        <v>218</v>
       </c>
       <c r="R67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="S67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>146</v>
+        <v>610</v>
       </c>
       <c r="T67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>71</v>
+        <v>513</v>
       </c>
       <c r="U67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>431</v>
+        <v>221</v>
       </c>
       <c r="V67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>527</v>
+        <v>690</v>
       </c>
       <c r="W67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>672</v>
+        <v>566</v>
       </c>
       <c r="X67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>408</v>
+        <v>313</v>
       </c>
       <c r="Y67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>441</v>
+        <v>161</v>
       </c>
       <c r="Z67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>299</v>
+        <v>653</v>
       </c>
       <c r="AA67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="AB67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>560</v>
+        <v>208</v>
       </c>
       <c r="AC67" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>399</v>
+        <v>634</v>
       </c>
     </row>
     <row r="68" spans="3:29" x14ac:dyDescent="0.25">
@@ -15035,7 +15037,7 @@
       </c>
       <c r="D68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>166</v>
+        <v>500</v>
       </c>
       <c r="E68" s="1">
         <f t="shared" ca="1" si="13"/>
@@ -15043,7 +15045,7 @@
       </c>
       <c r="F68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>724</v>
+        <v>675</v>
       </c>
       <c r="G68" s="1">
         <f t="shared" ca="1" si="13"/>
@@ -15051,7 +15053,7 @@
       </c>
       <c r="H68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>629</v>
+        <v>458</v>
       </c>
       <c r="I68" s="1">
         <f t="shared" ca="1" si="13"/>
@@ -15059,7 +15061,7 @@
       </c>
       <c r="J68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>259</v>
+        <v>381</v>
       </c>
       <c r="K68" s="1">
         <f t="shared" ca="1" si="13"/>
@@ -15067,7 +15069,7 @@
       </c>
       <c r="L68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="M68" s="1">
         <f t="shared" ca="1" si="13"/>
@@ -15075,67 +15077,67 @@
       </c>
       <c r="N68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>424</v>
+        <v>341</v>
       </c>
       <c r="O68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>86</v>
+        <v>317</v>
       </c>
       <c r="P68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="Q68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>263</v>
+        <v>516</v>
       </c>
       <c r="R68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>332</v>
+        <v>237</v>
       </c>
       <c r="S68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>394</v>
+        <v>91</v>
       </c>
       <c r="T68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>173</v>
+        <v>323</v>
       </c>
       <c r="U68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>471</v>
+        <v>587</v>
       </c>
       <c r="V68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>536</v>
+        <v>692</v>
       </c>
       <c r="W68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="X68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>206</v>
+        <v>646</v>
       </c>
       <c r="Y68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>728</v>
+        <v>586</v>
       </c>
       <c r="Z68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="AA68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>305</v>
+        <v>549</v>
       </c>
       <c r="AB68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>608</v>
+        <v>294</v>
       </c>
       <c r="AC68" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" spans="3:29" x14ac:dyDescent="0.25">
@@ -15145,7 +15147,7 @@
       </c>
       <c r="D69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>20</v>
+        <v>318</v>
       </c>
       <c r="E69" s="1">
         <f t="shared" ca="1" si="14"/>
@@ -15153,7 +15155,7 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>92</v>
+        <v>605</v>
       </c>
       <c r="G69" s="1">
         <f t="shared" ca="1" si="14"/>
@@ -15161,7 +15163,7 @@
       </c>
       <c r="H69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>479</v>
+        <v>212</v>
       </c>
       <c r="I69" s="1">
         <f t="shared" ca="1" si="14"/>
@@ -15169,7 +15171,7 @@
       </c>
       <c r="J69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>609</v>
+        <v>274</v>
       </c>
       <c r="K69" s="1">
         <f t="shared" ca="1" si="14"/>
@@ -15177,7 +15179,7 @@
       </c>
       <c r="L69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>429</v>
+        <v>660</v>
       </c>
       <c r="M69" s="1">
         <f t="shared" ca="1" si="14"/>
@@ -15185,67 +15187,67 @@
       </c>
       <c r="N69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>144</v>
+        <v>518</v>
       </c>
       <c r="O69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>678</v>
+        <v>486</v>
       </c>
       <c r="P69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>609</v>
+        <v>49</v>
       </c>
       <c r="Q69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>496</v>
+        <v>168</v>
       </c>
       <c r="R69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>695</v>
+        <v>253</v>
       </c>
       <c r="S69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>206</v>
+        <v>65</v>
       </c>
       <c r="T69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>500</v>
+        <v>178</v>
       </c>
       <c r="U69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>312</v>
+        <v>89</v>
       </c>
       <c r="V69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>341</v>
+        <v>312</v>
       </c>
       <c r="W69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>326</v>
+        <v>453</v>
       </c>
       <c r="X69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>634</v>
+        <v>450</v>
       </c>
       <c r="Y69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>198</v>
+        <v>396</v>
       </c>
       <c r="Z69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>260</v>
+        <v>64</v>
       </c>
       <c r="AA69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>157</v>
+        <v>720</v>
       </c>
       <c r="AB69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>504</v>
+        <v>723</v>
       </c>
       <c r="AC69" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>564</v>
+        <v>662</v>
       </c>
     </row>
     <row r="70" spans="3:29" x14ac:dyDescent="0.25">
@@ -15263,7 +15265,7 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>716</v>
+        <v>455</v>
       </c>
       <c r="G70" s="1">
         <f t="shared" ca="1" si="15"/>
@@ -15279,7 +15281,7 @@
       </c>
       <c r="J70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>210</v>
+        <v>124</v>
       </c>
       <c r="K70" s="1">
         <f t="shared" ca="1" si="15"/>
@@ -15295,93 +15297,93 @@
       </c>
       <c r="N70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>511</v>
+        <v>205</v>
       </c>
       <c r="O70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>212</v>
+        <v>261</v>
       </c>
       <c r="P70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>237</v>
+        <v>324</v>
       </c>
       <c r="Q70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>512</v>
+        <v>232</v>
       </c>
       <c r="R70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>376</v>
+        <v>169</v>
       </c>
       <c r="S70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>244</v>
+        <v>355</v>
       </c>
       <c r="T70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>273</v>
+        <v>601</v>
       </c>
       <c r="U70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>402</v>
+        <v>444</v>
       </c>
       <c r="V70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>632</v>
+        <v>95</v>
       </c>
       <c r="W70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="X70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>325</v>
+        <v>566</v>
       </c>
       <c r="Y70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>139</v>
+        <v>310</v>
       </c>
       <c r="Z70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>190</v>
+        <v>598</v>
       </c>
       <c r="AA70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="AB70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>615</v>
+        <v>711</v>
       </c>
       <c r="AC70" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>279</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
         <f t="shared" ref="C71:AC71" ca="1" si="16">IFERROR(CODE(LOWER(C42)),RANDBETWEEN(1,729))</f>
-        <v>527</v>
+        <v>567</v>
       </c>
       <c r="D71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>341</v>
+        <v>209</v>
       </c>
       <c r="E71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>370</v>
+        <v>98</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>237</v>
+        <v>496</v>
       </c>
       <c r="G71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>642</v>
+        <v>122</v>
       </c>
       <c r="H71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>296</v>
+        <v>508</v>
       </c>
       <c r="I71" s="1">
         <f t="shared" ca="1" si="16"/>
@@ -15393,105 +15395,105 @@
       </c>
       <c r="K71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="L71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>596</v>
+        <v>309</v>
       </c>
       <c r="M71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>367</v>
+        <v>656</v>
       </c>
       <c r="N71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="O71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>662</v>
+        <v>583</v>
       </c>
       <c r="P71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>405</v>
+        <v>292</v>
       </c>
       <c r="Q71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>560</v>
+        <v>715</v>
       </c>
       <c r="R71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>493</v>
+        <v>169</v>
       </c>
       <c r="S71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>703</v>
+        <v>126</v>
       </c>
       <c r="T71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>369</v>
+        <v>59</v>
       </c>
       <c r="U71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>640</v>
+        <v>44</v>
       </c>
       <c r="V71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>650</v>
+        <v>146</v>
       </c>
       <c r="W71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>624</v>
+        <v>430</v>
       </c>
       <c r="X71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>186</v>
+        <v>421</v>
       </c>
       <c r="Y71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>447</v>
+        <v>148</v>
       </c>
       <c r="Z71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="AA71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>720</v>
+        <v>385</v>
       </c>
       <c r="AB71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>663</v>
+        <v>708</v>
       </c>
       <c r="AC71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>574</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
         <f t="shared" ref="C72:AC72" ca="1" si="17">IFERROR(CODE(LOWER(C43)),RANDBETWEEN(1,729))</f>
-        <v>654</v>
+        <v>381</v>
       </c>
       <c r="D72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>446</v>
+        <v>643</v>
       </c>
       <c r="E72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>244</v>
+        <v>340</v>
       </c>
       <c r="F72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>722</v>
+        <v>575</v>
       </c>
       <c r="G72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>323</v>
+        <v>248</v>
       </c>
       <c r="H72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>200</v>
+        <v>674</v>
       </c>
       <c r="I72" s="1">
         <f t="shared" ca="1" si="17"/>
@@ -15499,109 +15501,109 @@
       </c>
       <c r="J72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>342</v>
+        <v>160</v>
       </c>
       <c r="K72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>315</v>
+        <v>185</v>
       </c>
       <c r="L72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>391</v>
+        <v>422</v>
       </c>
       <c r="M72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>458</v>
+        <v>47</v>
       </c>
       <c r="N72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>538</v>
+        <v>27</v>
       </c>
       <c r="O72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>673</v>
+        <v>37</v>
       </c>
       <c r="P72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>611</v>
+        <v>113</v>
       </c>
       <c r="Q72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>161</v>
+        <v>547</v>
       </c>
       <c r="R72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>273</v>
+        <v>444</v>
       </c>
       <c r="S72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>728</v>
+        <v>171</v>
       </c>
       <c r="T72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>187</v>
+        <v>308</v>
       </c>
       <c r="U72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>242</v>
+        <v>332</v>
       </c>
       <c r="V72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>171</v>
+        <v>606</v>
       </c>
       <c r="W72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>89</v>
+        <v>424</v>
       </c>
       <c r="X72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>277</v>
+        <v>438</v>
       </c>
       <c r="Y72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>556</v>
+        <v>219</v>
       </c>
       <c r="Z72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>2</v>
+        <v>402</v>
       </c>
       <c r="AA72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>474</v>
+        <v>161</v>
       </c>
       <c r="AB72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>489</v>
+        <v>437</v>
       </c>
       <c r="AC72" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>544</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
         <f t="shared" ref="C73:AC73" ca="1" si="18">IFERROR(CODE(LOWER(C44)),RANDBETWEEN(1,729))</f>
-        <v>321</v>
+        <v>706</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>379</v>
+        <v>277</v>
       </c>
       <c r="E73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>667</v>
+        <v>725</v>
       </c>
       <c r="F73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>277</v>
+        <v>38</v>
       </c>
       <c r="G73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>266</v>
+        <v>625</v>
       </c>
       <c r="H73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>588</v>
+        <v>309</v>
       </c>
       <c r="I73" s="1">
         <f t="shared" ca="1" si="18"/>
@@ -15609,105 +15611,105 @@
       </c>
       <c r="J73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>727</v>
+        <v>207</v>
       </c>
       <c r="K73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>57</v>
+        <v>279</v>
       </c>
       <c r="L73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>36</v>
+        <v>348</v>
       </c>
       <c r="M73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>681</v>
+        <v>148</v>
       </c>
       <c r="N73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>72</v>
+        <v>373</v>
       </c>
       <c r="O73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>581</v>
+        <v>354</v>
       </c>
       <c r="P73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>636</v>
+        <v>395</v>
       </c>
       <c r="Q73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="R73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>309</v>
+        <v>716</v>
       </c>
       <c r="S73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>573</v>
+        <v>491</v>
       </c>
       <c r="T73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>338</v>
+        <v>685</v>
       </c>
       <c r="U73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>84</v>
+        <v>486</v>
       </c>
       <c r="V73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>275</v>
+        <v>532</v>
       </c>
       <c r="W73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>132</v>
+        <v>316</v>
       </c>
       <c r="X73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="Y73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>176</v>
+        <v>570</v>
       </c>
       <c r="Z73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>59</v>
+        <v>440</v>
       </c>
       <c r="AA73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>299</v>
+        <v>479</v>
       </c>
       <c r="AB73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>370</v>
+        <v>98</v>
       </c>
       <c r="AC73" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>349</v>
+        <v>635</v>
       </c>
     </row>
     <row r="74" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
         <f t="shared" ref="C74:AC74" ca="1" si="19">IFERROR(CODE(LOWER(C45)),RANDBETWEEN(1,729))</f>
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="D74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>642</v>
+        <v>466</v>
       </c>
       <c r="E74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>153</v>
+        <v>384</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>651</v>
+        <v>242</v>
       </c>
       <c r="G74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>312</v>
+        <v>179</v>
       </c>
       <c r="H74" s="1">
         <f t="shared" ca="1" si="19"/>
@@ -15723,97 +15725,97 @@
       </c>
       <c r="K74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>550</v>
+        <v>486</v>
       </c>
       <c r="L74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>381</v>
+        <v>589</v>
       </c>
       <c r="M74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>248</v>
+        <v>15</v>
       </c>
       <c r="N74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="O74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>583</v>
+        <v>614</v>
       </c>
       <c r="P74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>700</v>
+        <v>316</v>
       </c>
       <c r="Q74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>649</v>
+        <v>261</v>
       </c>
       <c r="R74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>556</v>
+        <v>378</v>
       </c>
       <c r="S74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>477</v>
+        <v>451</v>
       </c>
       <c r="T74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>482</v>
+        <v>290</v>
       </c>
       <c r="U74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>466</v>
+        <v>156</v>
       </c>
       <c r="V74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>92</v>
+        <v>215</v>
       </c>
       <c r="W74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>215</v>
+        <v>655</v>
       </c>
       <c r="X74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>29</v>
+        <v>374</v>
       </c>
       <c r="Y74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>601</v>
+        <v>542</v>
       </c>
       <c r="Z74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>31</v>
+        <v>156</v>
       </c>
       <c r="AA74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="AB74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>664</v>
+        <v>292</v>
       </c>
       <c r="AC74" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>161</v>
+        <v>416</v>
       </c>
     </row>
     <row r="75" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
         <f t="shared" ref="C75:AC75" ca="1" si="20">IFERROR(CODE(LOWER(C46)),RANDBETWEEN(1,729))</f>
-        <v>563</v>
+        <v>527</v>
       </c>
       <c r="D75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>459</v>
+        <v>598</v>
       </c>
       <c r="E75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>273</v>
+        <v>230</v>
       </c>
       <c r="F75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>25</v>
+        <v>685</v>
       </c>
       <c r="G75" s="1">
         <f t="shared" ca="1" si="20"/>
@@ -15825,11 +15827,11 @@
       </c>
       <c r="I75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>633</v>
+        <v>505</v>
       </c>
       <c r="K75" s="1">
         <f t="shared" ca="1" si="20"/>
@@ -15841,85 +15843,85 @@
       </c>
       <c r="M75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>425</v>
+        <v>703</v>
       </c>
       <c r="N75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>392</v>
+        <v>318</v>
       </c>
       <c r="O75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>378</v>
+        <v>396</v>
       </c>
       <c r="P75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="Q75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>365</v>
+        <v>283</v>
       </c>
       <c r="R75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>369</v>
+        <v>626</v>
       </c>
       <c r="S75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>384</v>
+        <v>233</v>
       </c>
       <c r="T75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>351</v>
+        <v>235</v>
       </c>
       <c r="U75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>215</v>
+        <v>378</v>
       </c>
       <c r="V75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>425</v>
+        <v>452</v>
       </c>
       <c r="W75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>227</v>
+        <v>137</v>
       </c>
       <c r="X75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>435</v>
+        <v>530</v>
       </c>
       <c r="Y75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>51</v>
+        <v>192</v>
       </c>
       <c r="Z75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>107</v>
+        <v>362</v>
       </c>
       <c r="AA75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>614</v>
+        <v>163</v>
       </c>
       <c r="AB75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>238</v>
+        <v>347</v>
       </c>
       <c r="AC75" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>300</v>
+        <v>687</v>
       </c>
     </row>
     <row r="76" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
         <f t="shared" ref="C76:AC76" ca="1" si="21">IFERROR(CODE(LOWER(C47)),RANDBETWEEN(1,729))</f>
-        <v>112</v>
+        <v>666</v>
       </c>
       <c r="D76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="E76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>406</v>
+        <v>31</v>
       </c>
       <c r="F76" s="1">
         <f t="shared" ca="1" si="21"/>
@@ -15931,19 +15933,19 @@
       </c>
       <c r="H76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>104</v>
+        <v>198</v>
       </c>
       <c r="I76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>273</v>
+        <v>686</v>
       </c>
       <c r="J76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>530</v>
+        <v>441</v>
       </c>
       <c r="K76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>385</v>
+        <v>231</v>
       </c>
       <c r="L76" s="1">
         <f t="shared" ca="1" si="21"/>
@@ -15955,81 +15957,81 @@
       </c>
       <c r="N76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>157</v>
+        <v>381</v>
       </c>
       <c r="O76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>9</v>
+        <v>717</v>
       </c>
       <c r="P76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="Q76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>450</v>
+        <v>648</v>
       </c>
       <c r="R76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>176</v>
+        <v>554</v>
       </c>
       <c r="S76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="T76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>376</v>
+        <v>496</v>
       </c>
       <c r="U76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>91</v>
+        <v>437</v>
       </c>
       <c r="V76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>259</v>
+        <v>539</v>
       </c>
       <c r="W76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="X76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>696</v>
+        <v>475</v>
       </c>
       <c r="Y76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>606</v>
+        <v>292</v>
       </c>
       <c r="Z76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>150</v>
+        <v>687</v>
       </c>
       <c r="AA76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>110</v>
+        <v>612</v>
       </c>
       <c r="AB76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>679</v>
+        <v>169</v>
       </c>
       <c r="AC76" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>63</v>
+        <v>649</v>
       </c>
     </row>
     <row r="77" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
         <f t="shared" ref="C77:AC77" ca="1" si="22">IFERROR(CODE(LOWER(C48)),RANDBETWEEN(1,729))</f>
-        <v>568</v>
+        <v>699</v>
       </c>
       <c r="D77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>328</v>
+        <v>532</v>
       </c>
       <c r="E77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>587</v>
+        <v>251</v>
       </c>
       <c r="F77" s="1">
         <f t="shared" ca="1" si="22"/>
@@ -16037,27 +16039,27 @@
       </c>
       <c r="G77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>678</v>
+        <v>393</v>
       </c>
       <c r="H77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>242</v>
+        <v>24</v>
       </c>
       <c r="I77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="J77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>426</v>
+        <v>516</v>
       </c>
       <c r="K77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>694</v>
+        <v>214</v>
       </c>
       <c r="L77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>684</v>
+        <v>555</v>
       </c>
       <c r="M77" s="1">
         <f t="shared" ca="1" si="22"/>
@@ -16065,77 +16067,77 @@
       </c>
       <c r="N77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>399</v>
+        <v>164</v>
       </c>
       <c r="O77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>272</v>
+        <v>558</v>
       </c>
       <c r="P77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="Q77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="R77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>316</v>
+        <v>563</v>
       </c>
       <c r="S77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>630</v>
+        <v>659</v>
       </c>
       <c r="T77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="U77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>559</v>
+        <v>308</v>
       </c>
       <c r="V77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="W77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>229</v>
+        <v>617</v>
       </c>
       <c r="X77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="Y77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>594</v>
+        <v>178</v>
       </c>
       <c r="Z77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>687</v>
+        <v>423</v>
       </c>
       <c r="AA77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>100</v>
+        <v>493</v>
       </c>
       <c r="AB77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>698</v>
+        <v>310</v>
       </c>
       <c r="AC77" s="1">
         <f t="shared" ca="1" si="22"/>
-        <v>327</v>
+        <v>625</v>
       </c>
     </row>
     <row r="78" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <f t="shared" ref="C78:AC78" ca="1" si="23">IFERROR(CODE(LOWER(C49)),RANDBETWEEN(1,729))</f>
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>267</v>
+        <v>206</v>
       </c>
       <c r="E78" s="1">
         <f t="shared" ca="1" si="23"/>
@@ -16147,27 +16149,27 @@
       </c>
       <c r="G78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>94</v>
+        <v>714</v>
       </c>
       <c r="H78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>420</v>
+        <v>259</v>
       </c>
       <c r="I78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>458</v>
+        <v>587</v>
       </c>
       <c r="J78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>527</v>
+        <v>727</v>
       </c>
       <c r="K78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>373</v>
+        <v>220</v>
       </c>
       <c r="L78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>15</v>
+        <v>559</v>
       </c>
       <c r="M78" s="1">
         <f t="shared" ca="1" si="23"/>
@@ -16179,63 +16181,63 @@
       </c>
       <c r="O78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>204</v>
+        <v>67</v>
       </c>
       <c r="P78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>273</v>
+        <v>56</v>
       </c>
       <c r="Q78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>551</v>
+        <v>684</v>
       </c>
       <c r="R78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>43</v>
+        <v>217</v>
       </c>
       <c r="S78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>606</v>
+        <v>182</v>
       </c>
       <c r="T78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>226</v>
+        <v>554</v>
       </c>
       <c r="U78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="V78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>630</v>
+        <v>179</v>
       </c>
       <c r="W78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>377</v>
+        <v>432</v>
       </c>
       <c r="X78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>94</v>
+        <v>249</v>
       </c>
       <c r="Y78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="Z78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="AA78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>297</v>
+        <v>124</v>
       </c>
       <c r="AB78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>303</v>
+        <v>675</v>
       </c>
       <c r="AC78" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>459</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="3:29" x14ac:dyDescent="0.25">
@@ -16297,1045 +16299,1045 @@
       </c>
       <c r="Q79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>259</v>
+        <v>355</v>
       </c>
       <c r="R79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>269</v>
+        <v>438</v>
       </c>
       <c r="S79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>17</v>
+        <v>673</v>
       </c>
       <c r="T79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>492</v>
+        <v>342</v>
       </c>
       <c r="U79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>669</v>
+        <v>331</v>
       </c>
       <c r="V79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>389</v>
+        <v>184</v>
       </c>
       <c r="W79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>356</v>
+        <v>452</v>
       </c>
       <c r="X79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>381</v>
+        <v>729</v>
       </c>
       <c r="Y79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>16</v>
+        <v>542</v>
       </c>
       <c r="Z79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>286</v>
+        <v>54</v>
       </c>
       <c r="AA79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>567</v>
+        <v>354</v>
       </c>
       <c r="AB79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>478</v>
+        <v>433</v>
       </c>
       <c r="AC79" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>522</v>
+        <v>328</v>
       </c>
     </row>
     <row r="80" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <f t="shared" ref="C80:AC80" ca="1" si="25">IFERROR(CODE(LOWER(C51)),RANDBETWEEN(1,729))</f>
-        <v>506</v>
+        <v>419</v>
       </c>
       <c r="D80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>538</v>
+        <v>578</v>
       </c>
       <c r="E80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>377</v>
+        <v>562</v>
       </c>
       <c r="F80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>266</v>
+        <v>62</v>
       </c>
       <c r="G80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>692</v>
+        <v>479</v>
       </c>
       <c r="H80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>76</v>
+        <v>433</v>
       </c>
       <c r="I80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>352</v>
+        <v>590</v>
       </c>
       <c r="J80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>97</v>
+        <v>695</v>
       </c>
       <c r="K80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>35</v>
+        <v>586</v>
       </c>
       <c r="L80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>282</v>
+        <v>360</v>
       </c>
       <c r="M80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>308</v>
+        <v>359</v>
       </c>
       <c r="N80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>385</v>
+        <v>153</v>
       </c>
       <c r="O80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>94</v>
+        <v>687</v>
       </c>
       <c r="P80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>379</v>
+        <v>478</v>
       </c>
       <c r="Q80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>582</v>
+        <v>188</v>
       </c>
       <c r="R80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>520</v>
+        <v>305</v>
       </c>
       <c r="S80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>106</v>
+        <v>691</v>
       </c>
       <c r="T80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>30</v>
+        <v>279</v>
       </c>
       <c r="U80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>436</v>
+        <v>592</v>
       </c>
       <c r="V80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>454</v>
+        <v>519</v>
       </c>
       <c r="W80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>718</v>
+        <v>357</v>
       </c>
       <c r="X80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>272</v>
+        <v>663</v>
       </c>
       <c r="Y80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>511</v>
+        <v>206</v>
       </c>
       <c r="Z80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>390</v>
+        <v>713</v>
       </c>
       <c r="AA80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>683</v>
+        <v>509</v>
       </c>
       <c r="AB80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>218</v>
+        <v>93</v>
       </c>
       <c r="AC80" s="1">
         <f t="shared" ca="1" si="25"/>
-        <v>344</v>
+        <v>365</v>
       </c>
     </row>
     <row r="81" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <f t="shared" ref="C81:AC81" ca="1" si="26">IFERROR(CODE(LOWER(C52)),RANDBETWEEN(1,729))</f>
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="D81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>631</v>
+        <v>558</v>
       </c>
       <c r="E81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>272</v>
+        <v>304</v>
       </c>
       <c r="F81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>624</v>
+        <v>247</v>
       </c>
       <c r="G81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="H81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>213</v>
+        <v>276</v>
       </c>
       <c r="I81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>578</v>
+        <v>80</v>
       </c>
       <c r="J81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>238</v>
+        <v>618</v>
       </c>
       <c r="K81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>260</v>
+        <v>540</v>
       </c>
       <c r="L81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>482</v>
+        <v>575</v>
       </c>
       <c r="M81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>398</v>
+        <v>183</v>
       </c>
       <c r="N81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>342</v>
+        <v>51</v>
       </c>
       <c r="O81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>227</v>
+        <v>393</v>
       </c>
       <c r="P81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>614</v>
+        <v>416</v>
       </c>
       <c r="Q81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>692</v>
+        <v>222</v>
       </c>
       <c r="R81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>283</v>
+        <v>630</v>
       </c>
       <c r="S81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>700</v>
+        <v>468</v>
       </c>
       <c r="T81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>378</v>
+        <v>425</v>
       </c>
       <c r="U81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>636</v>
+        <v>144</v>
       </c>
       <c r="V81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>109</v>
+        <v>468</v>
       </c>
       <c r="W81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>262</v>
+        <v>191</v>
       </c>
       <c r="X81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="Y81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="Z81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>531</v>
+        <v>448</v>
       </c>
       <c r="AA81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>713</v>
+        <v>373</v>
       </c>
       <c r="AB81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>50</v>
+        <v>190</v>
       </c>
       <c r="AC81" s="1">
         <f t="shared" ca="1" si="26"/>
-        <v>32</v>
+        <v>345</v>
       </c>
     </row>
     <row r="82" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <f t="shared" ref="C82:AC82" ca="1" si="27">IFERROR(CODE(LOWER(C53)),RANDBETWEEN(1,729))</f>
-        <v>638</v>
+        <v>499</v>
       </c>
       <c r="D82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>533</v>
+        <v>718</v>
       </c>
       <c r="E82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>226</v>
+        <v>426</v>
       </c>
       <c r="F82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>539</v>
+        <v>8</v>
       </c>
       <c r="G82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>405</v>
+        <v>621</v>
       </c>
       <c r="H82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>386</v>
+        <v>299</v>
       </c>
       <c r="I82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>541</v>
+        <v>596</v>
       </c>
       <c r="J82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>684</v>
+        <v>281</v>
       </c>
       <c r="K82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>451</v>
+        <v>685</v>
       </c>
       <c r="L82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>430</v>
+        <v>363</v>
       </c>
       <c r="M82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>468</v>
+        <v>512</v>
       </c>
       <c r="N82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>374</v>
+        <v>621</v>
       </c>
       <c r="O82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>416</v>
+        <v>327</v>
       </c>
       <c r="P82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>461</v>
+        <v>115</v>
       </c>
       <c r="Q82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>388</v>
+        <v>304</v>
       </c>
       <c r="R82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="S82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>620</v>
+        <v>321</v>
       </c>
       <c r="T82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>594</v>
+        <v>514</v>
       </c>
       <c r="U82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>133</v>
+        <v>339</v>
       </c>
       <c r="V82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="W82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>724</v>
+        <v>102</v>
       </c>
       <c r="X82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>666</v>
+        <v>234</v>
       </c>
       <c r="Y82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>93</v>
+        <v>260</v>
       </c>
       <c r="Z82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>546</v>
+        <v>178</v>
       </c>
       <c r="AA82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>728</v>
+        <v>56</v>
       </c>
       <c r="AB82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>492</v>
+        <v>714</v>
       </c>
       <c r="AC82" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>75</v>
+        <v>210</v>
       </c>
     </row>
     <row r="83" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
         <f t="shared" ref="C83:AC83" ca="1" si="28">IFERROR(CODE(LOWER(C54)),RANDBETWEEN(1,729))</f>
-        <v>703</v>
+        <v>714</v>
       </c>
       <c r="D83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="E83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>340</v>
+        <v>287</v>
       </c>
       <c r="F83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>47</v>
+        <v>655</v>
       </c>
       <c r="H83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>398</v>
+        <v>315</v>
       </c>
       <c r="I83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>283</v>
+        <v>333</v>
       </c>
       <c r="J83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>404</v>
+        <v>515</v>
       </c>
       <c r="K83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="L83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>605</v>
+        <v>700</v>
       </c>
       <c r="M83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>331</v>
+        <v>266</v>
       </c>
       <c r="N83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>693</v>
+        <v>647</v>
       </c>
       <c r="O83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>598</v>
+        <v>685</v>
       </c>
       <c r="P83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>392</v>
+        <v>335</v>
       </c>
       <c r="Q83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>501</v>
+        <v>403</v>
       </c>
       <c r="R83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>258</v>
+        <v>522</v>
       </c>
       <c r="S83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>574</v>
+        <v>405</v>
       </c>
       <c r="T83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>522</v>
+        <v>439</v>
       </c>
       <c r="U83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>408</v>
+        <v>691</v>
       </c>
       <c r="V83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>300</v>
+        <v>728</v>
       </c>
       <c r="W83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>520</v>
+        <v>714</v>
       </c>
       <c r="X83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>705</v>
+        <v>454</v>
       </c>
       <c r="Y83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>549</v>
+        <v>349</v>
       </c>
       <c r="Z83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>472</v>
+        <v>42</v>
       </c>
       <c r="AA83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>5</v>
+        <v>256</v>
       </c>
       <c r="AB83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>656</v>
+        <v>671</v>
       </c>
       <c r="AC83" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>680</v>
+        <v>349</v>
       </c>
     </row>
     <row r="84" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
         <f t="shared" ref="C84:AC84" ca="1" si="29">IFERROR(CODE(LOWER(C55)),RANDBETWEEN(1,729))</f>
-        <v>630</v>
+        <v>342</v>
       </c>
       <c r="D84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>583</v>
+        <v>348</v>
       </c>
       <c r="E84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>382</v>
+        <v>422</v>
       </c>
       <c r="F84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>575</v>
+        <v>257</v>
       </c>
       <c r="G84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>368</v>
+        <v>420</v>
       </c>
       <c r="H84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>417</v>
+        <v>291</v>
       </c>
       <c r="I84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>584</v>
+        <v>448</v>
       </c>
       <c r="J84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>137</v>
+        <v>304</v>
       </c>
       <c r="K84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>259</v>
+        <v>471</v>
       </c>
       <c r="L84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>307</v>
       </c>
       <c r="M84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>178</v>
+        <v>218</v>
       </c>
       <c r="N84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>180</v>
+        <v>97</v>
       </c>
       <c r="O84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>555</v>
+        <v>714</v>
       </c>
       <c r="P84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>391</v>
+        <v>202</v>
       </c>
       <c r="Q84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>551</v>
+        <v>416</v>
       </c>
       <c r="R84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>188</v>
+        <v>641</v>
       </c>
       <c r="S84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>100</v>
+        <v>228</v>
       </c>
       <c r="T84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>641</v>
+        <v>666</v>
       </c>
       <c r="U84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>61</v>
+        <v>446</v>
       </c>
       <c r="V84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>269</v>
+        <v>507</v>
       </c>
       <c r="W84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="X84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>631</v>
+        <v>341</v>
       </c>
       <c r="Y84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>419</v>
+        <v>68</v>
       </c>
       <c r="Z84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>356</v>
+        <v>493</v>
       </c>
       <c r="AA84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>541</v>
+        <v>126</v>
       </c>
       <c r="AB84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>712</v>
+        <v>300</v>
       </c>
       <c r="AC84" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>644</v>
+        <v>365</v>
       </c>
     </row>
     <row r="85" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <f t="shared" ref="C85:AC85" ca="1" si="30">IFERROR(CODE(LOWER(C56)),RANDBETWEEN(1,729))</f>
-        <v>643</v>
+        <v>615</v>
       </c>
       <c r="D85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>240</v>
+        <v>376</v>
       </c>
       <c r="E85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>291</v>
+        <v>641</v>
       </c>
       <c r="F85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>74</v>
+        <v>408</v>
       </c>
       <c r="G85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="H85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>658</v>
+        <v>143</v>
       </c>
       <c r="I85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>602</v>
+        <v>184</v>
       </c>
       <c r="J85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>226</v>
+        <v>713</v>
       </c>
       <c r="K85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>676</v>
+        <v>415</v>
       </c>
       <c r="L85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="M85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>182</v>
+        <v>683</v>
       </c>
       <c r="N85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>441</v>
+        <v>688</v>
       </c>
       <c r="O85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>442</v>
+        <v>510</v>
       </c>
       <c r="P85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>13</v>
+        <v>208</v>
       </c>
       <c r="Q85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>290</v>
+        <v>559</v>
       </c>
       <c r="R85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>187</v>
+        <v>551</v>
       </c>
       <c r="S85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>691</v>
+        <v>580</v>
       </c>
       <c r="T85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>76</v>
+        <v>311</v>
       </c>
       <c r="U85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="V85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>482</v>
+        <v>44</v>
       </c>
       <c r="W85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>417</v>
+        <v>705</v>
       </c>
       <c r="X85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="Y85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>247</v>
+        <v>13</v>
       </c>
       <c r="Z85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>559</v>
+        <v>589</v>
       </c>
       <c r="AA85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>642</v>
+        <v>321</v>
       </c>
       <c r="AB85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="AC85" s="1">
         <f t="shared" ca="1" si="30"/>
-        <v>516</v>
+        <v>593</v>
       </c>
     </row>
     <row r="86" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <f t="shared" ref="C86:AC86" ca="1" si="31">IFERROR(CODE(LOWER(C57)),RANDBETWEEN(1,729))</f>
-        <v>604</v>
+        <v>46</v>
       </c>
       <c r="D86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>337</v>
+        <v>503</v>
       </c>
       <c r="E86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>429</v>
+        <v>83</v>
       </c>
       <c r="F86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>142</v>
+        <v>610</v>
       </c>
       <c r="G86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>621</v>
+        <v>542</v>
       </c>
       <c r="H86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>135</v>
+        <v>700</v>
       </c>
       <c r="I86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>364</v>
+        <v>18</v>
       </c>
       <c r="J86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>676</v>
+        <v>185</v>
       </c>
       <c r="K86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>129</v>
+        <v>558</v>
       </c>
       <c r="L86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>421</v>
+        <v>333</v>
       </c>
       <c r="M86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>382</v>
+        <v>500</v>
       </c>
       <c r="N86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>357</v>
+        <v>471</v>
       </c>
       <c r="O86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>411</v>
+        <v>593</v>
       </c>
       <c r="P86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>560</v>
+        <v>328</v>
       </c>
       <c r="Q86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>411</v>
+        <v>530</v>
       </c>
       <c r="R86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>200</v>
+        <v>542</v>
       </c>
       <c r="S86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>61</v>
+        <v>601</v>
       </c>
       <c r="T86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>143</v>
+        <v>269</v>
       </c>
       <c r="U86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="V86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>331</v>
+        <v>284</v>
       </c>
       <c r="W86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>175</v>
+        <v>482</v>
       </c>
       <c r="X86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>725</v>
+        <v>146</v>
       </c>
       <c r="Y86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>703</v>
+        <v>435</v>
       </c>
       <c r="Z86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>331</v>
+        <v>501</v>
       </c>
       <c r="AA86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>176</v>
+        <v>343</v>
       </c>
       <c r="AB86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>477</v>
+        <v>645</v>
       </c>
       <c r="AC86" s="1">
         <f t="shared" ca="1" si="31"/>
-        <v>351</v>
+        <v>662</v>
       </c>
     </row>
     <row r="87" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <f t="shared" ref="C87:AC87" ca="1" si="32">IFERROR(CODE(LOWER(C58)),RANDBETWEEN(1,729))</f>
-        <v>695</v>
+        <v>270</v>
       </c>
       <c r="D87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="E87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>161</v>
+        <v>589</v>
       </c>
       <c r="F87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>405</v>
+        <v>459</v>
       </c>
       <c r="G87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>280</v>
+        <v>162</v>
       </c>
       <c r="H87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>410</v>
+        <v>726</v>
       </c>
       <c r="I87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>693</v>
+        <v>216</v>
       </c>
       <c r="J87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>328</v>
+        <v>28</v>
       </c>
       <c r="K87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>639</v>
+        <v>115</v>
       </c>
       <c r="L87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>336</v>
+        <v>536</v>
       </c>
       <c r="M87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>6</v>
+        <v>655</v>
       </c>
       <c r="N87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>164</v>
+        <v>568</v>
       </c>
       <c r="O87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>117</v>
+        <v>440</v>
       </c>
       <c r="P87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>478</v>
+        <v>19</v>
       </c>
       <c r="Q87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>98</v>
+        <v>664</v>
       </c>
       <c r="R87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="S87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>61</v>
+        <v>516</v>
       </c>
       <c r="T87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>642</v>
+        <v>277</v>
       </c>
       <c r="U87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>633</v>
+        <v>214</v>
       </c>
       <c r="V87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="W87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>676</v>
+        <v>392</v>
       </c>
       <c r="X87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>411</v>
+        <v>654</v>
       </c>
       <c r="Y87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>99</v>
+        <v>355</v>
       </c>
       <c r="Z87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>155</v>
+        <v>289</v>
       </c>
       <c r="AA87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>669</v>
+        <v>636</v>
       </c>
       <c r="AB87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>683</v>
+        <v>148</v>
       </c>
       <c r="AC87" s="1">
         <f t="shared" ca="1" si="32"/>
-        <v>489</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <f t="shared" ref="C88:AC88" ca="1" si="33">IFERROR(CODE(LOWER(C59)),RANDBETWEEN(1,729))</f>
-        <v>373</v>
+        <v>426</v>
       </c>
       <c r="D88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>93</v>
+        <v>402</v>
       </c>
       <c r="E88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>56</v>
+        <v>249</v>
       </c>
       <c r="F88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>62</v>
+        <v>212</v>
       </c>
       <c r="G88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>539</v>
+        <v>147</v>
       </c>
       <c r="H88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>467</v>
+        <v>239</v>
       </c>
       <c r="I88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>331</v>
+        <v>241</v>
       </c>
       <c r="J88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>277</v>
+        <v>709</v>
       </c>
       <c r="K88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="L88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>132</v>
+        <v>667</v>
       </c>
       <c r="M88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>162</v>
+        <v>347</v>
       </c>
       <c r="N88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>550</v>
+        <v>460</v>
       </c>
       <c r="O88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>117</v>
+        <v>700</v>
       </c>
       <c r="P88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>425</v>
+        <v>501</v>
       </c>
       <c r="Q88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>583</v>
+        <v>677</v>
       </c>
       <c r="R88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>659</v>
+        <v>667</v>
       </c>
       <c r="S88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>401</v>
+        <v>497</v>
       </c>
       <c r="T88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>724</v>
+        <v>8</v>
       </c>
       <c r="U88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>590</v>
+        <v>123</v>
       </c>
       <c r="V88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="W88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>342</v>
+        <v>573</v>
       </c>
       <c r="X88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>185</v>
+        <v>87</v>
       </c>
       <c r="Y88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>206</v>
+        <v>728</v>
       </c>
       <c r="Z88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="AA88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>679</v>
+        <v>640</v>
       </c>
       <c r="AB88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>390</v>
+        <v>253</v>
       </c>
       <c r="AC88" s="1">
         <f t="shared" ca="1" si="33"/>
-        <v>665</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>